<commit_message>
Primera iteración entregada y aprobada
</commit_message>
<xml_diff>
--- a/Anexos/Métricas.xlsx
+++ b/Anexos/Métricas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alumnosuaiedu-my.sharepoint.com/personal/ignacioadriel_roldanfarias_alumnos_uai_edu_ar/Documents/Desktop/Facu - copia/2025 1er cuatri/Proyecto/Primera Iteracion/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alumnosuaiedu-my.sharepoint.com/personal/ignacioadriel_roldanfarias_alumnos_uai_edu_ar/Documents/Desktop/Facu - copia/2025 1er cuatri/Proyecto/Primera Iteracion/Anexos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="133" documentId="8_{DF3D1BE8-4A93-4ED3-A826-1E34E96FC085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E20A610B-D770-42A8-8522-7DCADA6C35E3}"/>
+  <xr:revisionPtr revIDLastSave="135" documentId="8_{DF3D1BE8-4A93-4ED3-A826-1E34E96FC085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D62417A4-F0F5-4711-A768-608A4360BB19}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="656" firstSheet="3" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Proyecto" sheetId="8" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="Parámetros" sheetId="6" r:id="rId8"/>
     <sheet name="Aplanamiento" sheetId="14" r:id="rId9"/>
     <sheet name="Factores Calculo" sheetId="15" r:id="rId10"/>
+    <sheet name="Hoja1" sheetId="16" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="5">'Ajustes Ambientales'!$A$1:$H$20</definedName>
@@ -4327,6 +4328,299 @@
     <xf numFmtId="0" fontId="49" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="41" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="4" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="4" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="4" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="4" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="4" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="4" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="34" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4371,304 +4665,11 @@
     <xf numFmtId="0" fontId="43" fillId="23" borderId="38" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="41" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="4" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="4" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="4" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="4" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="4" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="4" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="51" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -4770,10 +4771,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5066,8 +5063,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5080,12 +5077,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="225" t="s">
+      <c r="A1" s="223" t="s">
         <v>290</v>
       </c>
-      <c r="B1" s="226"/>
-      <c r="C1" s="226"/>
-      <c r="D1" s="227"/>
+      <c r="B1" s="224"/>
+      <c r="C1" s="224"/>
+      <c r="D1" s="225"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33"/>
@@ -5094,24 +5091,24 @@
       <c r="D2" s="36"/>
     </row>
     <row r="3" spans="1:8" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="240" t="s">
+      <c r="A3" s="238" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="241"/>
-      <c r="C3" s="241"/>
-      <c r="D3" s="242"/>
+      <c r="B3" s="239"/>
+      <c r="C3" s="239"/>
+      <c r="D3" s="240"/>
       <c r="E3" s="37"/>
       <c r="F3" s="38"/>
       <c r="G3" s="38"/>
       <c r="H3" s="38"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="243" t="s">
+      <c r="A4" s="241" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="244"/>
-      <c r="C4" s="244"/>
-      <c r="D4" s="245"/>
+      <c r="B4" s="242"/>
+      <c r="C4" s="242"/>
+      <c r="D4" s="243"/>
       <c r="E4" s="37"/>
       <c r="F4" s="38"/>
       <c r="G4" s="38"/>
@@ -5121,11 +5118,11 @@
       <c r="A5" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="228" t="s">
+      <c r="B5" s="226" t="s">
         <v>329</v>
       </c>
-      <c r="C5" s="229"/>
-      <c r="D5" s="230"/>
+      <c r="C5" s="227"/>
+      <c r="D5" s="228"/>
       <c r="E5" s="37"/>
       <c r="F5" s="38"/>
       <c r="G5" s="38"/>
@@ -5135,29 +5132,29 @@
       <c r="A6" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="228" t="s">
+      <c r="B6" s="226" t="s">
         <v>330</v>
       </c>
-      <c r="C6" s="229"/>
-      <c r="D6" s="230"/>
+      <c r="C6" s="227"/>
+      <c r="D6" s="228"/>
       <c r="E6" s="37"/>
       <c r="F6" s="38"/>
       <c r="G6" s="38"/>
       <c r="H6" s="38"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="231" t="s">
+      <c r="A7" s="229" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="232"/>
-      <c r="C7" s="232"/>
-      <c r="D7" s="233"/>
+      <c r="B7" s="230"/>
+      <c r="C7" s="230"/>
+      <c r="D7" s="231"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="325" t="s">
+      <c r="B8" s="211" t="s">
         <v>331</v>
       </c>
       <c r="C8" s="25" t="s">
@@ -5169,100 +5166,108 @@
       <c r="A9" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="234" t="s">
+      <c r="B9" s="232" t="s">
         <v>332</v>
       </c>
-      <c r="C9" s="235"/>
-      <c r="D9" s="236"/>
+      <c r="C9" s="233"/>
+      <c r="D9" s="234"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="237" t="s">
+      <c r="A10" s="235" t="s">
         <v>66</v>
       </c>
-      <c r="B10" s="238"/>
-      <c r="C10" s="238"/>
-      <c r="D10" s="239"/>
+      <c r="B10" s="236"/>
+      <c r="C10" s="236"/>
+      <c r="D10" s="237"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="40" t="s">
         <v>100</v>
       </c>
-      <c r="B11" s="246"/>
-      <c r="C11" s="247"/>
-      <c r="D11" s="248"/>
+      <c r="B11" s="212"/>
+      <c r="C11" s="213"/>
+      <c r="D11" s="214"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="B12" s="249"/>
-      <c r="C12" s="247"/>
-      <c r="D12" s="248"/>
+      <c r="B12" s="215"/>
+      <c r="C12" s="213"/>
+      <c r="D12" s="214"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="B13" s="246"/>
-      <c r="C13" s="247"/>
-      <c r="D13" s="248"/>
+      <c r="B13" s="212"/>
+      <c r="C13" s="213"/>
+      <c r="D13" s="214"/>
     </row>
     <row r="14" spans="1:8" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="250"/>
-      <c r="C14" s="251"/>
-      <c r="D14" s="252"/>
+      <c r="B14" s="216"/>
+      <c r="C14" s="217"/>
+      <c r="D14" s="218"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="254" t="s">
+      <c r="A18" s="220" t="s">
         <v>86</v>
       </c>
-      <c r="B18" s="255"/>
-      <c r="C18" s="255"/>
-      <c r="D18" s="256"/>
+      <c r="B18" s="221"/>
+      <c r="C18" s="221"/>
+      <c r="D18" s="222"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="71" t="s">
         <v>87</v>
       </c>
-      <c r="B19" s="249" t="s">
+      <c r="B19" s="215" t="s">
         <v>333</v>
       </c>
-      <c r="C19" s="247"/>
-      <c r="D19" s="248"/>
+      <c r="C19" s="213"/>
+      <c r="D19" s="214"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="71" t="s">
         <v>88</v>
       </c>
-      <c r="B20" s="249" t="s">
+      <c r="B20" s="215" t="s">
         <v>333</v>
       </c>
-      <c r="C20" s="247"/>
-      <c r="D20" s="248"/>
+      <c r="C20" s="213"/>
+      <c r="D20" s="214"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="71" t="s">
         <v>68</v>
       </c>
-      <c r="B21" s="249" t="s">
+      <c r="B21" s="215" t="s">
         <v>333</v>
       </c>
-      <c r="C21" s="247"/>
-      <c r="D21" s="248"/>
+      <c r="C21" s="213"/>
+      <c r="D21" s="214"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="71" t="s">
         <v>89</v>
       </c>
-      <c r="B22" s="253"/>
-      <c r="C22" s="247"/>
-      <c r="D22" s="248"/>
+      <c r="B22" s="219"/>
+      <c r="C22" s="213"/>
+      <c r="D22" s="214"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="B5:D5"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
@@ -5272,14 +5277,6 @@
     <mergeCell ref="B19:D19"/>
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="B21:D21"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="B5:D5"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.23622047244094491" right="0.27" top="0.51" bottom="0.43307086614173229" header="0.11811023622047245" footer="0.23622047244094491"/>
@@ -5308,23 +5305,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="320" t="s">
+      <c r="A1" s="324" t="s">
         <v>212</v>
       </c>
-      <c r="B1" s="320"/>
-      <c r="C1" s="320"/>
-      <c r="D1" s="320"/>
-      <c r="E1" s="320"/>
+      <c r="B1" s="324"/>
+      <c r="C1" s="324"/>
+      <c r="D1" s="324"/>
+      <c r="E1" s="324"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="319" t="s">
+      <c r="A2" s="325" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="319"/>
-      <c r="D2" s="319" t="s">
+      <c r="B2" s="325"/>
+      <c r="D2" s="325" t="s">
         <v>58</v>
       </c>
-      <c r="E2" s="319"/>
+      <c r="E2" s="325"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="195" t="s">
@@ -5412,14 +5409,14 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="319" t="s">
+      <c r="A10" s="325" t="s">
         <v>162</v>
       </c>
-      <c r="B10" s="319"/>
-      <c r="D10" s="319" t="s">
+      <c r="B10" s="325"/>
+      <c r="D10" s="325" t="s">
         <v>163</v>
       </c>
-      <c r="E10" s="319"/>
+      <c r="E10" s="325"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="196" t="s">
@@ -5506,14 +5503,14 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="319" t="s">
+      <c r="A18" s="325" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="319"/>
-      <c r="D18" s="319" t="s">
+      <c r="B18" s="325"/>
+      <c r="D18" s="325" t="s">
         <v>164</v>
       </c>
-      <c r="E18" s="319"/>
+      <c r="E18" s="325"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="196" t="s">
@@ -5600,14 +5597,14 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="319" t="s">
+      <c r="A26" s="325" t="s">
         <v>57</v>
       </c>
-      <c r="B26" s="319"/>
-      <c r="D26" s="319" t="s">
+      <c r="B26" s="325"/>
+      <c r="D26" s="325" t="s">
         <v>59</v>
       </c>
-      <c r="E26" s="319"/>
+      <c r="E26" s="325"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
@@ -5694,23 +5691,23 @@
       </c>
     </row>
     <row r="35" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="320" t="s">
+      <c r="A35" s="324" t="s">
         <v>213</v>
       </c>
-      <c r="B35" s="320"/>
-      <c r="C35" s="320"/>
-      <c r="D35" s="320"/>
-      <c r="E35" s="320"/>
+      <c r="B35" s="324"/>
+      <c r="C35" s="324"/>
+      <c r="D35" s="324"/>
+      <c r="E35" s="324"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="319" t="s">
+      <c r="A36" s="325" t="s">
         <v>214</v>
       </c>
-      <c r="B36" s="319"/>
-      <c r="D36" s="319" t="s">
+      <c r="B36" s="325"/>
+      <c r="D36" s="325" t="s">
         <v>53</v>
       </c>
-      <c r="E36" s="319"/>
+      <c r="E36" s="325"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="196" t="s">
@@ -5797,14 +5794,14 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="319" t="s">
+      <c r="A44" s="325" t="s">
         <v>221</v>
       </c>
-      <c r="B44" s="319"/>
-      <c r="D44" s="319" t="s">
+      <c r="B44" s="325"/>
+      <c r="D44" s="325" t="s">
         <v>263</v>
       </c>
-      <c r="E44" s="319"/>
+      <c r="E44" s="325"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
@@ -5891,14 +5888,14 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="319" t="s">
+      <c r="A52" s="325" t="s">
         <v>228</v>
       </c>
-      <c r="B52" s="319"/>
-      <c r="D52" s="319" t="s">
+      <c r="B52" s="325"/>
+      <c r="D52" s="325" t="s">
         <v>54</v>
       </c>
-      <c r="E52" s="319"/>
+      <c r="E52" s="325"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="196" t="s">
@@ -5985,14 +5982,14 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="319" t="s">
+      <c r="A60" s="325" t="s">
         <v>229</v>
       </c>
-      <c r="B60" s="319"/>
-      <c r="D60" s="319" t="s">
+      <c r="B60" s="325"/>
+      <c r="D60" s="325" t="s">
         <v>276</v>
       </c>
-      <c r="E60" s="319"/>
+      <c r="E60" s="325"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
@@ -6079,14 +6076,14 @@
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="319" t="s">
+      <c r="A68" s="325" t="s">
         <v>236</v>
       </c>
-      <c r="B68" s="319"/>
-      <c r="D68" s="319" t="s">
+      <c r="B68" s="325"/>
+      <c r="D68" s="325" t="s">
         <v>165</v>
       </c>
-      <c r="E68" s="319"/>
+      <c r="E68" s="325"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
@@ -6173,14 +6170,14 @@
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="319" t="s">
+      <c r="A76" s="325" t="s">
         <v>243</v>
       </c>
-      <c r="B76" s="319"/>
-      <c r="D76" s="319" t="s">
+      <c r="B76" s="325"/>
+      <c r="D76" s="325" t="s">
         <v>166</v>
       </c>
-      <c r="E76" s="319"/>
+      <c r="E76" s="325"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
@@ -6267,10 +6264,10 @@
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" s="319" t="s">
+      <c r="A84" s="325" t="s">
         <v>250</v>
       </c>
-      <c r="B84" s="319"/>
+      <c r="B84" s="325"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
@@ -6323,6 +6320,16 @@
   </sheetData>
   <sheetProtection password="F673" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="23">
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="A60:B60"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A35:E35"/>
     <mergeCell ref="A36:B36"/>
@@ -6336,16 +6343,6 @@
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="D26:E26"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="A60:B60"/>
   </mergeCells>
   <conditionalFormatting sqref="G3">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
@@ -6362,6 +6359,18 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72FE0F23-77A7-4B9C-9C50-AF5ACBE9E276}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -6382,32 +6391,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="257" t="s">
+      <c r="A1" s="250" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="257"/>
-      <c r="C1" s="257"/>
-      <c r="D1" s="257"/>
-      <c r="E1" s="257"/>
-      <c r="F1" s="257"/>
-      <c r="G1" s="257"/>
-      <c r="H1" s="257"/>
-      <c r="I1" s="257"/>
-      <c r="J1" s="257"/>
+      <c r="B1" s="250"/>
+      <c r="C1" s="250"/>
+      <c r="D1" s="250"/>
+      <c r="E1" s="250"/>
+      <c r="F1" s="250"/>
+      <c r="G1" s="250"/>
+      <c r="H1" s="250"/>
+      <c r="I1" s="250"/>
+      <c r="J1" s="250"/>
     </row>
     <row r="2" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="257" t="s">
+      <c r="A2" s="250" t="s">
         <v>99</v>
       </c>
-      <c r="B2" s="257"/>
-      <c r="C2" s="257"/>
-      <c r="D2" s="257"/>
-      <c r="E2" s="257"/>
-      <c r="F2" s="257"/>
-      <c r="G2" s="257"/>
-      <c r="H2" s="257"/>
-      <c r="I2" s="257"/>
-      <c r="J2" s="257"/>
+      <c r="B2" s="250"/>
+      <c r="C2" s="250"/>
+      <c r="D2" s="250"/>
+      <c r="E2" s="250"/>
+      <c r="F2" s="250"/>
+      <c r="G2" s="250"/>
+      <c r="H2" s="250"/>
+      <c r="I2" s="250"/>
+      <c r="J2" s="250"/>
     </row>
     <row r="4" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="43"/>
@@ -6424,148 +6433,148 @@
       <c r="J5" s="46"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="262" t="s">
+      <c r="B6" s="253" t="s">
         <v>70</v>
       </c>
-      <c r="C6" s="263"/>
-      <c r="D6" s="263"/>
-      <c r="E6" s="263"/>
-      <c r="F6" s="263"/>
-      <c r="G6" s="263"/>
-      <c r="H6" s="263"/>
-      <c r="I6" s="263"/>
-      <c r="J6" s="264"/>
+      <c r="C6" s="254"/>
+      <c r="D6" s="254"/>
+      <c r="E6" s="254"/>
+      <c r="F6" s="254"/>
+      <c r="G6" s="254"/>
+      <c r="H6" s="254"/>
+      <c r="I6" s="254"/>
+      <c r="J6" s="255"/>
     </row>
     <row r="7" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
-      <c r="C7" s="258" t="s">
+      <c r="C7" s="246" t="s">
         <v>71</v>
       </c>
-      <c r="D7" s="258"/>
-      <c r="E7" s="258"/>
-      <c r="F7" s="258"/>
-      <c r="G7" s="258"/>
-      <c r="H7" s="258"/>
-      <c r="I7" s="258"/>
-      <c r="J7" s="259"/>
+      <c r="D7" s="246"/>
+      <c r="E7" s="246"/>
+      <c r="F7" s="246"/>
+      <c r="G7" s="246"/>
+      <c r="H7" s="246"/>
+      <c r="I7" s="246"/>
+      <c r="J7" s="247"/>
     </row>
     <row r="8" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="265" t="s">
+      <c r="B8" s="256" t="s">
         <v>98</v>
       </c>
-      <c r="C8" s="266"/>
-      <c r="D8" s="266"/>
-      <c r="E8" s="266"/>
-      <c r="F8" s="266"/>
-      <c r="G8" s="266"/>
-      <c r="H8" s="266"/>
-      <c r="I8" s="266"/>
-      <c r="J8" s="267"/>
+      <c r="C8" s="257"/>
+      <c r="D8" s="257"/>
+      <c r="E8" s="257"/>
+      <c r="F8" s="257"/>
+      <c r="G8" s="257"/>
+      <c r="H8" s="257"/>
+      <c r="I8" s="257"/>
+      <c r="J8" s="258"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="47" t="s">
         <v>72</v>
       </c>
-      <c r="C9" s="268" t="s">
+      <c r="C9" s="259" t="s">
         <v>73</v>
       </c>
-      <c r="D9" s="269"/>
-      <c r="E9" s="269"/>
-      <c r="F9" s="269"/>
-      <c r="G9" s="269"/>
-      <c r="H9" s="269"/>
-      <c r="I9" s="269"/>
-      <c r="J9" s="270"/>
+      <c r="D9" s="260"/>
+      <c r="E9" s="260"/>
+      <c r="F9" s="260"/>
+      <c r="G9" s="260"/>
+      <c r="H9" s="260"/>
+      <c r="I9" s="260"/>
+      <c r="J9" s="261"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="258" t="s">
+      <c r="C10" s="246" t="s">
         <v>74</v>
       </c>
-      <c r="D10" s="258"/>
-      <c r="E10" s="258"/>
-      <c r="F10" s="258"/>
-      <c r="G10" s="258"/>
-      <c r="H10" s="258"/>
-      <c r="I10" s="258"/>
-      <c r="J10" s="259"/>
+      <c r="D10" s="246"/>
+      <c r="E10" s="246"/>
+      <c r="F10" s="246"/>
+      <c r="G10" s="246"/>
+      <c r="H10" s="246"/>
+      <c r="I10" s="246"/>
+      <c r="J10" s="247"/>
     </row>
     <row r="11" spans="1:10" ht="78" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C11" s="273" t="s">
+      <c r="C11" s="248" t="s">
         <v>76</v>
       </c>
-      <c r="D11" s="273"/>
-      <c r="E11" s="273"/>
-      <c r="F11" s="273"/>
-      <c r="G11" s="273"/>
-      <c r="H11" s="273"/>
-      <c r="I11" s="273"/>
-      <c r="J11" s="274"/>
+      <c r="D11" s="248"/>
+      <c r="E11" s="248"/>
+      <c r="F11" s="248"/>
+      <c r="G11" s="248"/>
+      <c r="H11" s="248"/>
+      <c r="I11" s="248"/>
+      <c r="J11" s="249"/>
     </row>
     <row r="12" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C12" s="273" t="s">
+      <c r="C12" s="248" t="s">
         <v>77</v>
       </c>
-      <c r="D12" s="273"/>
-      <c r="E12" s="273"/>
-      <c r="F12" s="273"/>
-      <c r="G12" s="273"/>
-      <c r="H12" s="273"/>
-      <c r="I12" s="273"/>
-      <c r="J12" s="274"/>
+      <c r="D12" s="248"/>
+      <c r="E12" s="248"/>
+      <c r="F12" s="248"/>
+      <c r="G12" s="248"/>
+      <c r="H12" s="248"/>
+      <c r="I12" s="248"/>
+      <c r="J12" s="249"/>
     </row>
     <row r="13" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C13" s="258" t="s">
+      <c r="C13" s="246" t="s">
         <v>79</v>
       </c>
-      <c r="D13" s="258"/>
-      <c r="E13" s="258"/>
-      <c r="F13" s="258"/>
-      <c r="G13" s="258"/>
-      <c r="H13" s="258"/>
-      <c r="I13" s="258"/>
-      <c r="J13" s="259"/>
+      <c r="D13" s="246"/>
+      <c r="E13" s="246"/>
+      <c r="F13" s="246"/>
+      <c r="G13" s="246"/>
+      <c r="H13" s="246"/>
+      <c r="I13" s="246"/>
+      <c r="J13" s="247"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C14" s="258" t="s">
+      <c r="C14" s="246" t="s">
         <v>81</v>
       </c>
-      <c r="D14" s="258"/>
-      <c r="E14" s="258"/>
-      <c r="F14" s="258"/>
-      <c r="G14" s="258"/>
-      <c r="H14" s="258"/>
-      <c r="I14" s="258"/>
-      <c r="J14" s="259"/>
+      <c r="D14" s="246"/>
+      <c r="E14" s="246"/>
+      <c r="F14" s="246"/>
+      <c r="G14" s="246"/>
+      <c r="H14" s="246"/>
+      <c r="I14" s="246"/>
+      <c r="J14" s="247"/>
     </row>
     <row r="15" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="48" t="s">
         <v>80</v>
       </c>
-      <c r="C15" s="260" t="s">
+      <c r="C15" s="251" t="s">
         <v>82</v>
       </c>
-      <c r="D15" s="260"/>
-      <c r="E15" s="260"/>
-      <c r="F15" s="260"/>
-      <c r="G15" s="260"/>
-      <c r="H15" s="260"/>
-      <c r="I15" s="260"/>
-      <c r="J15" s="261"/>
+      <c r="D15" s="251"/>
+      <c r="E15" s="251"/>
+      <c r="F15" s="251"/>
+      <c r="G15" s="251"/>
+      <c r="H15" s="251"/>
+      <c r="I15" s="251"/>
+      <c r="J15" s="252"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C16" s="49"/>
@@ -6578,14 +6587,14 @@
       <c r="J16" s="49"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C17" s="271"/>
-      <c r="D17" s="271"/>
-      <c r="E17" s="271"/>
-      <c r="F17" s="271"/>
-      <c r="G17" s="271"/>
-      <c r="H17" s="271"/>
-      <c r="I17" s="271"/>
-      <c r="J17" s="271"/>
+      <c r="C17" s="244"/>
+      <c r="D17" s="244"/>
+      <c r="E17" s="244"/>
+      <c r="F17" s="244"/>
+      <c r="G17" s="244"/>
+      <c r="H17" s="244"/>
+      <c r="I17" s="244"/>
+      <c r="J17" s="244"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="50" t="s">
@@ -6612,26 +6621,20 @@
       <c r="I19" s="52"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="272" t="s">
+      <c r="B20" s="245" t="s">
         <v>85</v>
       </c>
-      <c r="C20" s="272"/>
-      <c r="D20" s="272"/>
-      <c r="E20" s="272"/>
-      <c r="F20" s="272"/>
-      <c r="G20" s="272"/>
-      <c r="H20" s="272"/>
-      <c r="I20" s="272"/>
+      <c r="C20" s="245"/>
+      <c r="D20" s="245"/>
+      <c r="E20" s="245"/>
+      <c r="F20" s="245"/>
+      <c r="G20" s="245"/>
+      <c r="H20" s="245"/>
+      <c r="I20" s="245"/>
     </row>
     <row r="22" spans="2:10" ht="107.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C17:J17"/>
-    <mergeCell ref="B20:I20"/>
-    <mergeCell ref="C10:J10"/>
-    <mergeCell ref="C11:J11"/>
-    <mergeCell ref="C12:J12"/>
-    <mergeCell ref="C13:J13"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="C14:J14"/>
@@ -6640,6 +6643,12 @@
     <mergeCell ref="C7:J7"/>
     <mergeCell ref="B8:J8"/>
     <mergeCell ref="C9:J9"/>
+    <mergeCell ref="C17:J17"/>
+    <mergeCell ref="B20:I20"/>
+    <mergeCell ref="C10:J10"/>
+    <mergeCell ref="C11:J11"/>
+    <mergeCell ref="C12:J12"/>
+    <mergeCell ref="C13:J13"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.23" right="0.27" top="0.46" bottom="0.69" header="0.2" footer="0.5"/>
@@ -6653,11 +6662,11 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet21"/>
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -6670,82 +6679,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="257" t="s">
+      <c r="A1" s="250" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="257"/>
-      <c r="C1" s="257"/>
-      <c r="D1" s="257"/>
-      <c r="E1" s="257"/>
+      <c r="B1" s="250"/>
+      <c r="C1" s="250"/>
+      <c r="D1" s="250"/>
+      <c r="E1" s="250"/>
     </row>
     <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="257" t="s">
+      <c r="A2" s="250" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="257"/>
-      <c r="C2" s="257"/>
-      <c r="D2" s="257"/>
-      <c r="E2" s="257"/>
+      <c r="B2" s="250"/>
+      <c r="C2" s="250"/>
+      <c r="D2" s="250"/>
+      <c r="E2" s="250"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C4" s="286" t="s">
+      <c r="C4" s="273" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="287"/>
-      <c r="E4" s="284">
+      <c r="D4" s="274"/>
+      <c r="E4" s="271">
         <f>Parámetros!E13</f>
         <v>2662</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C5" s="288"/>
-      <c r="D5" s="289"/>
-      <c r="E5" s="285"/>
+      <c r="C5" s="275"/>
+      <c r="D5" s="276"/>
+      <c r="E5" s="272"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C6" s="286" t="s">
+      <c r="C6" s="273" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="287"/>
-      <c r="E6" s="284">
+      <c r="D6" s="274"/>
+      <c r="E6" s="271">
         <f>Parámetros!E12</f>
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C7" s="288"/>
-      <c r="D7" s="289"/>
-      <c r="E7" s="285"/>
+      <c r="C7" s="275"/>
+      <c r="D7" s="276"/>
+      <c r="E7" s="272"/>
     </row>
     <row r="9" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="279" t="s">
+      <c r="A9" s="266" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="279"/>
-      <c r="C9" s="279"/>
-      <c r="D9" s="279"/>
-      <c r="E9" s="279"/>
+      <c r="B9" s="266"/>
+      <c r="C9" s="266"/>
+      <c r="D9" s="266"/>
+      <c r="E9" s="266"/>
     </row>
     <row r="10" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="277" t="s">
+      <c r="A10" s="264" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="278"/>
-      <c r="C10" s="278"/>
-      <c r="D10" s="278"/>
-      <c r="E10" s="278"/>
+      <c r="B10" s="265"/>
+      <c r="C10" s="265"/>
+      <c r="D10" s="265"/>
+      <c r="E10" s="265"/>
     </row>
     <row r="11" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="280" t="s">
+      <c r="A12" s="267" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="283"/>
-      <c r="C12" s="280" t="s">
+      <c r="B12" s="270"/>
+      <c r="C12" s="267" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="281"/>
-      <c r="E12" s="282"/>
+      <c r="D12" s="268"/>
+      <c r="E12" s="269"/>
     </row>
     <row r="13" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
@@ -6775,9 +6784,9 @@
       <c r="E14" s="60">
         <v>1</v>
       </c>
-      <c r="F14" s="102" t="str">
-        <f>IF(OR(AND(C19&lt;&gt;"",D14&lt;&gt;""),AND(C19&lt;&gt;"",E14&lt;&gt;""),AND(D14&lt;&gt;"",E14&lt;&gt;"")),"* Completar sólo 1 columna",(IF(OR(C19&gt;1,D14&gt;1,E14&gt;1),"* Se recomienda utilizar 1","")))</f>
-        <v/>
+      <c r="F14" s="102" t="e">
+        <f>IF(OR(AND(#REF!&lt;&gt;"",D14&lt;&gt;""),AND(#REF!&lt;&gt;"",E14&lt;&gt;""),AND(D14&lt;&gt;"",E14&lt;&gt;"")),"* Completar sólo 1 columna",(IF(OR(#REF!&gt;1,D14&gt;1,E14&gt;1),"* Se recomienda utilizar 1","")))</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
@@ -6793,7 +6802,7 @@
         <v>1</v>
       </c>
       <c r="F15" s="102" t="str">
-        <f t="shared" ref="F15:F35" si="0">IF(OR(AND(C15&lt;&gt;"",D15&lt;&gt;""),AND(C15&lt;&gt;"",E15&lt;&gt;""),AND(D15&lt;&gt;"",E15&lt;&gt;"")),"* Completar sólo 1 columna",(IF(OR(C15&gt;1,D15&gt;1,E15&gt;1),"* Se recomienda utilizar 1","")))</f>
+        <f t="shared" ref="F15:F18" si="0">IF(OR(AND(C15&lt;&gt;"",D15&lt;&gt;""),AND(C15&lt;&gt;"",E15&lt;&gt;""),AND(D15&lt;&gt;"",E15&lt;&gt;"")),"* Completar sólo 1 columna",(IF(OR(C15&gt;1,D15&gt;1,E15&gt;1),"* Se recomienda utilizar 1","")))</f>
         <v/>
       </c>
     </row>
@@ -6825,226 +6834,39 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="53"/>
       <c r="B18" s="54"/>
-      <c r="C18" s="58"/>
-      <c r="D18" s="59"/>
-      <c r="E18" s="60"/>
+      <c r="C18" s="55"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="57"/>
       <c r="F18" s="102" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="53"/>
-      <c r="B19" s="54"/>
-      <c r="C19" s="118"/>
-      <c r="D19" s="59"/>
-      <c r="E19" s="60"/>
-      <c r="F19" s="102" t="e">
-        <f>IF(OR(AND(#REF!&lt;&gt;"",D19&lt;&gt;""),AND(#REF!&lt;&gt;"",E19&lt;&gt;""),AND(D19&lt;&gt;"",E19&lt;&gt;"")),"* Completar sólo 1 columna",(IF(OR(#REF!&gt;1,D19&gt;1,E19&gt;1),"* Se recomienda utilizar 1","")))</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="53"/>
-      <c r="B20" s="54"/>
-      <c r="C20" s="58"/>
-      <c r="D20" s="59"/>
-      <c r="E20" s="60"/>
-      <c r="F20" s="102" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="53"/>
-      <c r="B21" s="54"/>
-      <c r="C21" s="58"/>
-      <c r="D21" s="59"/>
-      <c r="E21" s="60"/>
-      <c r="F21" s="102" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="53"/>
-      <c r="B22" s="54"/>
-      <c r="C22" s="58"/>
-      <c r="D22" s="59"/>
-      <c r="E22" s="60"/>
-      <c r="F22" s="102" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="53"/>
-      <c r="B23" s="54"/>
-      <c r="C23" s="58"/>
-      <c r="D23" s="59"/>
-      <c r="E23" s="60"/>
-      <c r="F23" s="102" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="53"/>
-      <c r="B24" s="54"/>
-      <c r="C24" s="58"/>
-      <c r="D24" s="59"/>
-      <c r="E24" s="60"/>
-      <c r="F24" s="102" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="53"/>
-      <c r="B25" s="54"/>
-      <c r="C25" s="58"/>
-      <c r="D25" s="59"/>
-      <c r="E25" s="60"/>
-      <c r="F25" s="102" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="53"/>
-      <c r="B26" s="54"/>
-      <c r="C26" s="55"/>
-      <c r="D26" s="56"/>
-      <c r="E26" s="57"/>
-      <c r="F26" s="102" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="53"/>
-      <c r="B27" s="54"/>
-      <c r="C27" s="55"/>
-      <c r="D27" s="56"/>
-      <c r="E27" s="57"/>
-      <c r="F27" s="102" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="53"/>
-      <c r="B28" s="54"/>
-      <c r="C28" s="55"/>
-      <c r="D28" s="56"/>
-      <c r="E28" s="57"/>
-      <c r="F28" s="102" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="53"/>
-      <c r="B29" s="54"/>
-      <c r="C29" s="55"/>
-      <c r="D29" s="56"/>
-      <c r="E29" s="57"/>
-      <c r="F29" s="102" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="53"/>
-      <c r="B30" s="54"/>
-      <c r="C30" s="55"/>
-      <c r="D30" s="56"/>
-      <c r="E30" s="57"/>
-      <c r="F30" s="102" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="53"/>
-      <c r="B31" s="54"/>
-      <c r="C31" s="55"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="57"/>
-      <c r="F31" s="102" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="53"/>
-      <c r="B32" s="54"/>
-      <c r="C32" s="55"/>
-      <c r="D32" s="56"/>
-      <c r="E32" s="57"/>
-      <c r="F32" s="102" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="53"/>
-      <c r="B33" s="54"/>
-      <c r="C33" s="55"/>
-      <c r="D33" s="56"/>
-      <c r="E33" s="57"/>
-      <c r="F33" s="102" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="53"/>
-      <c r="B34" s="54"/>
-      <c r="C34" s="55"/>
-      <c r="D34" s="56"/>
-      <c r="E34" s="57"/>
-      <c r="F34" s="102" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="53"/>
-      <c r="B35" s="54"/>
-      <c r="C35" s="55"/>
-      <c r="D35" s="56"/>
-      <c r="E35" s="57"/>
-      <c r="F35" s="102" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="275" t="s">
+    <row r="19" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="262" t="s">
         <v>3</v>
       </c>
-      <c r="B36" s="276"/>
-      <c r="C36" s="16">
-        <f>SUM(C15:C35)</f>
-        <v>0</v>
-      </c>
-      <c r="D36" s="16">
-        <f>SUM(D14:D35)</f>
-        <v>0</v>
-      </c>
-      <c r="E36" s="16">
-        <f>SUM(E14:E35)</f>
+      <c r="B19" s="263"/>
+      <c r="C19" s="16">
+        <f>SUM(C15:C18)</f>
+        <v>0</v>
+      </c>
+      <c r="D19" s="16">
+        <f>SUM(D14:D18)</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="16">
+        <f>SUM(E14:E18)</f>
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection insertColumns="0" insertRows="0" sort="0" autoFilter="0"/>
   <mergeCells count="11">
-    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A19:B19"/>
     <mergeCell ref="A10:E10"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
@@ -7073,8 +6895,8 @@
   <dimension ref="A1:N86"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
+      <pane ySplit="2" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -7087,13 +6909,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="257" t="s">
+      <c r="A1" s="250" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="257"/>
-      <c r="C1" s="257"/>
-      <c r="D1" s="257"/>
-      <c r="E1" s="257"/>
+      <c r="B1" s="250"/>
+      <c r="C1" s="250"/>
+      <c r="D1" s="250"/>
+      <c r="E1" s="250"/>
       <c r="F1" s="106"/>
       <c r="G1" s="106"/>
       <c r="H1" s="106"/>
@@ -7105,10 +6927,10 @@
       <c r="N1" s="106"/>
     </row>
     <row r="2" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="257" t="s">
+      <c r="A2" s="250" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="257"/>
+      <c r="B2" s="250"/>
       <c r="C2" s="106"/>
       <c r="D2" s="106"/>
       <c r="E2" s="106"/>
@@ -7131,105 +6953,105 @@
       <c r="F3" s="82"/>
     </row>
     <row r="4" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="286" t="s">
+      <c r="C4" s="273" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="287"/>
-      <c r="E4" s="284">
+      <c r="D4" s="274"/>
+      <c r="E4" s="271">
         <f>Parámetros!E13</f>
         <v>2662</v>
       </c>
       <c r="F4" s="88"/>
-      <c r="K4" s="286" t="s">
+      <c r="K4" s="273" t="s">
         <v>30</v>
       </c>
-      <c r="L4" s="287"/>
-      <c r="M4" s="284">
+      <c r="L4" s="274"/>
+      <c r="M4" s="271">
         <f>Parámetros!E13</f>
         <v>2662</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="288"/>
-      <c r="D5" s="289"/>
-      <c r="E5" s="285"/>
+      <c r="C5" s="275"/>
+      <c r="D5" s="276"/>
+      <c r="E5" s="272"/>
       <c r="F5" s="88"/>
-      <c r="K5" s="288"/>
-      <c r="L5" s="289"/>
-      <c r="M5" s="285"/>
+      <c r="K5" s="275"/>
+      <c r="L5" s="276"/>
+      <c r="M5" s="272"/>
     </row>
     <row r="6" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="286" t="s">
+      <c r="C6" s="273" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="287"/>
-      <c r="E6" s="284">
+      <c r="D6" s="274"/>
+      <c r="E6" s="271">
         <f>Parámetros!E12</f>
         <v>15</v>
       </c>
       <c r="F6" s="88"/>
-      <c r="K6" s="286" t="s">
+      <c r="K6" s="273" t="s">
         <v>31</v>
       </c>
-      <c r="L6" s="287"/>
-      <c r="M6" s="284">
+      <c r="L6" s="274"/>
+      <c r="M6" s="271">
         <f>Parámetros!E12</f>
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="288"/>
-      <c r="D7" s="289"/>
-      <c r="E7" s="285"/>
+      <c r="C7" s="275"/>
+      <c r="D7" s="276"/>
+      <c r="E7" s="272"/>
       <c r="F7" s="88"/>
-      <c r="K7" s="288"/>
-      <c r="L7" s="289"/>
-      <c r="M7" s="285"/>
+      <c r="K7" s="275"/>
+      <c r="L7" s="276"/>
+      <c r="M7" s="272"/>
     </row>
     <row r="9" spans="1:14" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="279" t="s">
+      <c r="A9" s="266" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="279"/>
-      <c r="C9" s="279"/>
-      <c r="D9" s="279"/>
-      <c r="E9" s="279"/>
+      <c r="B9" s="266"/>
+      <c r="C9" s="266"/>
+      <c r="D9" s="266"/>
+      <c r="E9" s="266"/>
       <c r="F9" s="89"/>
     </row>
     <row r="10" spans="1:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="277" t="s">
+      <c r="A10" s="264" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="278"/>
-      <c r="C10" s="278"/>
-      <c r="D10" s="278"/>
-      <c r="E10" s="278"/>
+      <c r="B10" s="265"/>
+      <c r="C10" s="265"/>
+      <c r="D10" s="265"/>
+      <c r="E10" s="265"/>
       <c r="F10" s="90"/>
     </row>
     <row r="11" spans="1:14" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F11" s="90"/>
     </row>
     <row r="12" spans="1:14" s="18" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="294" t="s">
+      <c r="A12" s="277" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="295"/>
-      <c r="C12" s="280" t="s">
+      <c r="B12" s="278"/>
+      <c r="C12" s="267" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="281"/>
-      <c r="E12" s="282"/>
+      <c r="D12" s="268"/>
+      <c r="E12" s="269"/>
       <c r="F12" s="90"/>
-      <c r="G12" s="290" t="s">
+      <c r="G12" s="279" t="s">
         <v>101</v>
       </c>
-      <c r="H12" s="291"/>
-      <c r="I12" s="291"/>
-      <c r="J12" s="291"/>
-      <c r="K12" s="291"/>
-      <c r="L12" s="291"/>
-      <c r="M12" s="291"/>
-      <c r="N12" s="292"/>
+      <c r="H12" s="280"/>
+      <c r="I12" s="280"/>
+      <c r="J12" s="280"/>
+      <c r="K12" s="280"/>
+      <c r="L12" s="280"/>
+      <c r="M12" s="280"/>
+      <c r="N12" s="281"/>
     </row>
     <row r="13" spans="1:14" s="18" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="119" t="s">
@@ -7280,7 +7102,7 @@
       <c r="B14" s="205" t="s">
         <v>292</v>
       </c>
-      <c r="C14" s="321">
+      <c r="C14" s="207">
         <v>1</v>
       </c>
       <c r="D14" s="59"/>
@@ -7516,11 +7338,11 @@
       <c r="B19" s="54" t="s">
         <v>305</v>
       </c>
-      <c r="C19" s="322"/>
-      <c r="D19" s="322">
+      <c r="C19" s="208"/>
+      <c r="D19" s="208">
         <v>1</v>
       </c>
-      <c r="E19" s="322"/>
+      <c r="E19" s="208"/>
       <c r="F19" s="116"/>
       <c r="G19" s="114">
         <f t="shared" si="0"/>
@@ -7562,9 +7384,9 @@
       <c r="B20" s="206" t="s">
         <v>306</v>
       </c>
-      <c r="C20" s="322"/>
-      <c r="D20" s="322"/>
-      <c r="E20" s="322">
+      <c r="C20" s="208"/>
+      <c r="D20" s="208"/>
+      <c r="E20" s="208">
         <v>1</v>
       </c>
       <c r="F20" s="116"/>
@@ -7608,11 +7430,11 @@
       <c r="B21" s="206" t="s">
         <v>308</v>
       </c>
-      <c r="C21" s="322"/>
-      <c r="D21" s="322">
+      <c r="C21" s="208"/>
+      <c r="D21" s="208">
         <v>1</v>
       </c>
-      <c r="E21" s="322"/>
+      <c r="E21" s="208"/>
       <c r="F21" s="116"/>
       <c r="G21" s="114">
         <f t="shared" si="0"/>
@@ -7654,11 +7476,11 @@
       <c r="B22" s="206" t="s">
         <v>309</v>
       </c>
-      <c r="C22" s="322"/>
-      <c r="D22" s="322">
+      <c r="C22" s="208"/>
+      <c r="D22" s="208">
         <v>1</v>
       </c>
-      <c r="E22" s="322"/>
+      <c r="E22" s="208"/>
       <c r="F22" s="116"/>
       <c r="G22" s="114">
         <f t="shared" si="0"/>
@@ -7700,9 +7522,9 @@
       <c r="B23" s="206" t="s">
         <v>310</v>
       </c>
-      <c r="C23" s="322"/>
-      <c r="D23" s="322"/>
-      <c r="E23" s="322">
+      <c r="C23" s="208"/>
+      <c r="D23" s="208"/>
+      <c r="E23" s="208">
         <v>1</v>
       </c>
       <c r="F23" s="116" t="str">
@@ -7745,9 +7567,9 @@
     <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="166"/>
       <c r="B24" s="206"/>
-      <c r="C24" s="322"/>
-      <c r="D24" s="322"/>
-      <c r="E24" s="322"/>
+      <c r="C24" s="208"/>
+      <c r="D24" s="208"/>
+      <c r="E24" s="208"/>
       <c r="F24" s="116"/>
       <c r="G24" s="114">
         <f t="shared" si="0"/>
@@ -7785,9 +7607,9 @@
     <row r="25" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A25" s="166"/>
       <c r="B25" s="200"/>
-      <c r="C25" s="322"/>
-      <c r="D25" s="322"/>
-      <c r="E25" s="322"/>
+      <c r="C25" s="208"/>
+      <c r="D25" s="208"/>
+      <c r="E25" s="208"/>
       <c r="F25" s="116" t="str">
         <f t="shared" ref="F25:F52" si="1">IF(OR(AND(C25&lt;&gt;"",D25&lt;&gt;""),AND(C25&lt;&gt;"",E25&lt;&gt;""),AND(D25&lt;&gt;"",E25&lt;&gt;"")),"Error: completar sólo 1 col.",(IF(OR(C25&gt;1,D25&gt;1,E25&gt;1),"Recomend: utilizar valor=1","")))</f>
         <v/>
@@ -9311,12 +9133,12 @@
       </c>
     </row>
     <row r="63" spans="1:14" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C63" s="293">
+      <c r="C63" s="282">
         <f>SUM(C62*5+D62*10+E62*15)</f>
         <v>115</v>
       </c>
-      <c r="D63" s="293"/>
-      <c r="E63" s="293"/>
+      <c r="D63" s="282"/>
+      <c r="E63" s="282"/>
       <c r="G63" s="107" t="s">
         <v>3</v>
       </c>
@@ -9460,13 +9282,6 @@
   </sheetData>
   <sheetProtection insertColumns="0" insertRows="0" sort="0"/>
   <mergeCells count="16">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A9:E9"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="C6:D7"/>
-    <mergeCell ref="A2:B2"/>
     <mergeCell ref="G12:N12"/>
     <mergeCell ref="C63:E63"/>
     <mergeCell ref="E6:E7"/>
@@ -9476,6 +9291,13 @@
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="K6:L7"/>
     <mergeCell ref="M6:M7"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="C6:D7"/>
+    <mergeCell ref="A2:B2"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="G14:N62">
@@ -9498,9 +9320,9 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="F1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -9515,31 +9337,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="257" t="s">
+      <c r="A1" s="250" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="257"/>
-      <c r="C1" s="257"/>
-      <c r="D1" s="257"/>
-      <c r="E1" s="257"/>
-      <c r="F1" s="257"/>
-      <c r="G1" s="257"/>
-      <c r="H1" s="257"/>
+      <c r="B1" s="250"/>
+      <c r="C1" s="250"/>
+      <c r="D1" s="250"/>
+      <c r="E1" s="250"/>
+      <c r="F1" s="250"/>
+      <c r="G1" s="250"/>
+      <c r="H1" s="250"/>
       <c r="I1" s="42"/>
       <c r="J1"/>
       <c r="K1"/>
     </row>
     <row r="2" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="257" t="s">
+      <c r="A2" s="250" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="257"/>
-      <c r="C2" s="257"/>
-      <c r="D2" s="257"/>
-      <c r="E2" s="257"/>
-      <c r="F2" s="257"/>
-      <c r="G2" s="257"/>
-      <c r="H2" s="257"/>
+      <c r="B2" s="250"/>
+      <c r="C2" s="250"/>
+      <c r="D2" s="250"/>
+      <c r="E2" s="250"/>
+      <c r="F2" s="250"/>
+      <c r="G2" s="250"/>
+      <c r="H2" s="250"/>
     </row>
     <row r="3" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="82"/>
@@ -9556,48 +9378,48 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C4" s="83"/>
-      <c r="D4" s="286" t="s">
+      <c r="D4" s="273" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="287"/>
+      <c r="E4" s="274"/>
       <c r="F4" s="192"/>
-      <c r="G4" s="284">
+      <c r="G4" s="271">
         <f>Parámetros!E13</f>
         <v>2662</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C5" s="83"/>
-      <c r="D5" s="288"/>
-      <c r="E5" s="289"/>
+      <c r="D5" s="275"/>
+      <c r="E5" s="276"/>
       <c r="F5" s="193"/>
-      <c r="G5" s="285"/>
+      <c r="G5" s="272"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C6" s="83"/>
-      <c r="D6" s="286" t="s">
+      <c r="D6" s="273" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="287"/>
+      <c r="E6" s="274"/>
       <c r="F6" s="192"/>
-      <c r="G6" s="284">
+      <c r="G6" s="271">
         <f>Parámetros!E12</f>
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C7" s="83"/>
-      <c r="D7" s="288"/>
-      <c r="E7" s="289"/>
+      <c r="D7" s="275"/>
+      <c r="E7" s="276"/>
       <c r="F7" s="193"/>
-      <c r="G7" s="285"/>
+      <c r="G7" s="272"/>
     </row>
     <row r="9" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="279"/>
-      <c r="B9" s="279"/>
-      <c r="C9" s="279"/>
-      <c r="D9" s="279"/>
-      <c r="E9" s="279"/>
+      <c r="A9" s="266"/>
+      <c r="B9" s="266"/>
+      <c r="C9" s="266"/>
+      <c r="D9" s="266"/>
+      <c r="E9" s="266"/>
       <c r="F9" s="191"/>
       <c r="G9" s="30"/>
       <c r="H9" s="31" t="s">
@@ -9606,11 +9428,11 @@
     </row>
     <row r="11" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:12" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="299" t="s">
+      <c r="A12" s="286" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="300"/>
-      <c r="C12" s="300"/>
+      <c r="B12" s="287"/>
+      <c r="C12" s="287"/>
       <c r="D12" s="27" t="s">
         <v>48</v>
       </c>
@@ -9632,11 +9454,11 @@
       <c r="L12" s="29"/>
     </row>
     <row r="13" spans="1:12" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="296" t="s">
+      <c r="A13" s="283" t="s">
         <v>286</v>
       </c>
-      <c r="B13" s="297"/>
-      <c r="C13" s="298"/>
+      <c r="B13" s="284"/>
+      <c r="C13" s="285"/>
       <c r="D13" s="61">
         <v>1</v>
       </c>
@@ -9651,17 +9473,17 @@
         <f>F13*D13</f>
         <v>2</v>
       </c>
-      <c r="H13" s="323" t="s">
+      <c r="H13" s="209" t="s">
         <v>316</v>
       </c>
       <c r="L13" s="28"/>
     </row>
     <row r="14" spans="1:12" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="296" t="s">
+      <c r="A14" s="283" t="s">
         <v>287</v>
       </c>
-      <c r="B14" s="297"/>
-      <c r="C14" s="298"/>
+      <c r="B14" s="284"/>
+      <c r="C14" s="285"/>
       <c r="D14" s="62">
         <v>1</v>
       </c>
@@ -9676,17 +9498,17 @@
         <f t="shared" ref="G14:G25" si="0">F14*D14</f>
         <v>2</v>
       </c>
-      <c r="H14" s="323" t="s">
+      <c r="H14" s="209" t="s">
         <v>317</v>
       </c>
       <c r="L14" s="28"/>
     </row>
     <row r="15" spans="1:12" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="296" t="s">
+      <c r="A15" s="283" t="s">
         <v>228</v>
       </c>
-      <c r="B15" s="297"/>
-      <c r="C15" s="298"/>
+      <c r="B15" s="284"/>
+      <c r="C15" s="285"/>
       <c r="D15" s="62">
         <v>4</v>
       </c>
@@ -9701,17 +9523,17 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="H15" s="323" t="s">
+      <c r="H15" s="209" t="s">
         <v>318</v>
       </c>
       <c r="L15" s="28"/>
     </row>
     <row r="16" spans="1:12" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="296" t="s">
+      <c r="A16" s="283" t="s">
         <v>229</v>
       </c>
-      <c r="B16" s="297"/>
-      <c r="C16" s="298"/>
+      <c r="B16" s="284"/>
+      <c r="C16" s="285"/>
       <c r="D16" s="62">
         <v>3</v>
       </c>
@@ -9726,17 +9548,17 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="H16" s="323" t="s">
+      <c r="H16" s="209" t="s">
         <v>319</v>
       </c>
       <c r="L16" s="28"/>
     </row>
     <row r="17" spans="1:12" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="296" t="s">
+      <c r="A17" s="283" t="s">
         <v>236</v>
       </c>
-      <c r="B17" s="297"/>
-      <c r="C17" s="298"/>
+      <c r="B17" s="284"/>
+      <c r="C17" s="285"/>
       <c r="D17" s="62">
         <v>3</v>
       </c>
@@ -9751,17 +9573,17 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="H17" s="323" t="s">
+      <c r="H17" s="209" t="s">
         <v>320</v>
       </c>
       <c r="L17" s="28"/>
     </row>
     <row r="18" spans="1:12" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="296" t="s">
+      <c r="A18" s="283" t="s">
         <v>243</v>
       </c>
-      <c r="B18" s="297"/>
-      <c r="C18" s="298"/>
+      <c r="B18" s="284"/>
+      <c r="C18" s="285"/>
       <c r="D18" s="62">
         <v>2</v>
       </c>
@@ -9776,17 +9598,17 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="H18" s="323" t="s">
+      <c r="H18" s="209" t="s">
         <v>321</v>
       </c>
       <c r="L18" s="28"/>
     </row>
     <row r="19" spans="1:12" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="296" t="s">
+      <c r="A19" s="283" t="s">
         <v>288</v>
       </c>
-      <c r="B19" s="297"/>
-      <c r="C19" s="298"/>
+      <c r="B19" s="284"/>
+      <c r="C19" s="285"/>
       <c r="D19" s="62">
         <v>4</v>
       </c>
@@ -9800,17 +9622,17 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="H19" s="323" t="s">
+      <c r="H19" s="209" t="s">
         <v>322</v>
       </c>
       <c r="L19" s="28"/>
     </row>
     <row r="20" spans="1:12" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="296" t="s">
+      <c r="A20" s="283" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="297"/>
-      <c r="C20" s="298"/>
+      <c r="B20" s="284"/>
+      <c r="C20" s="285"/>
       <c r="D20" s="62">
         <v>1</v>
       </c>
@@ -9825,17 +9647,17 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H20" s="323" t="s">
+      <c r="H20" s="209" t="s">
         <v>323</v>
       </c>
       <c r="L20" s="28"/>
     </row>
     <row r="21" spans="1:12" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="296" t="s">
+      <c r="A21" s="283" t="s">
         <v>285</v>
       </c>
-      <c r="B21" s="297"/>
-      <c r="C21" s="298"/>
+      <c r="B21" s="284"/>
+      <c r="C21" s="285"/>
       <c r="D21" s="62">
         <v>3</v>
       </c>
@@ -9850,17 +9672,17 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="H21" s="323" t="s">
+      <c r="H21" s="209" t="s">
         <v>324</v>
       </c>
       <c r="L21" s="28"/>
     </row>
     <row r="22" spans="1:12" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="296" t="s">
+      <c r="A22" s="283" t="s">
         <v>54</v>
       </c>
-      <c r="B22" s="297"/>
-      <c r="C22" s="298"/>
+      <c r="B22" s="284"/>
+      <c r="C22" s="285"/>
       <c r="D22" s="62">
         <v>2</v>
       </c>
@@ -9875,17 +9697,17 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="H22" s="323" t="s">
+      <c r="H22" s="209" t="s">
         <v>325</v>
       </c>
       <c r="L22" s="28"/>
     </row>
     <row r="23" spans="1:12" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="296" t="s">
+      <c r="A23" s="283" t="s">
         <v>276</v>
       </c>
-      <c r="B23" s="297"/>
-      <c r="C23" s="298"/>
+      <c r="B23" s="284"/>
+      <c r="C23" s="285"/>
       <c r="D23" s="62">
         <v>4</v>
       </c>
@@ -9900,17 +9722,17 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="H23" s="323" t="s">
+      <c r="H23" s="209" t="s">
         <v>326</v>
       </c>
       <c r="L23" s="28"/>
     </row>
     <row r="24" spans="1:12" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="296" t="s">
+      <c r="A24" s="283" t="s">
         <v>165</v>
       </c>
-      <c r="B24" s="297"/>
-      <c r="C24" s="298"/>
+      <c r="B24" s="284"/>
+      <c r="C24" s="285"/>
       <c r="D24" s="62">
         <v>0</v>
       </c>
@@ -9925,17 +9747,17 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H24" s="323" t="s">
+      <c r="H24" s="209" t="s">
         <v>327</v>
       </c>
       <c r="L24" s="28"/>
     </row>
     <row r="25" spans="1:12" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="296" t="s">
+      <c r="A25" s="283" t="s">
         <v>166</v>
       </c>
-      <c r="B25" s="297"/>
-      <c r="C25" s="298"/>
+      <c r="B25" s="284"/>
+      <c r="C25" s="285"/>
       <c r="D25" s="63">
         <v>1</v>
       </c>
@@ -9950,7 +9772,7 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="H25" s="323" t="s">
+      <c r="H25" s="209" t="s">
         <v>328</v>
       </c>
       <c r="L25" s="28"/>
@@ -9963,14 +9785,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="D4:E5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="D6:E7"/>
     <mergeCell ref="A16:C16"/>
     <mergeCell ref="A9:E9"/>
     <mergeCell ref="A24:C24"/>
@@ -9984,6 +9798,14 @@
     <mergeCell ref="A20:C20"/>
     <mergeCell ref="A19:C19"/>
     <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="D4:E5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="D6:E7"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.23622047244094491" right="0.2" top="0.46" bottom="0.35433070866141736" header="0.15748031496062992" footer="0.15748031496062992"/>
@@ -10102,28 +9924,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="257" t="s">
+      <c r="A1" s="250" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="301"/>
-      <c r="C1" s="301"/>
-      <c r="D1" s="301"/>
-      <c r="E1" s="301"/>
-      <c r="F1" s="301"/>
-      <c r="G1" s="301"/>
-      <c r="H1" s="301"/>
+      <c r="B1" s="290"/>
+      <c r="C1" s="290"/>
+      <c r="D1" s="290"/>
+      <c r="E1" s="290"/>
+      <c r="F1" s="290"/>
+      <c r="G1" s="290"/>
+      <c r="H1" s="290"/>
     </row>
     <row r="2" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="302" t="s">
+      <c r="A2" s="291" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="301"/>
-      <c r="C2" s="301"/>
-      <c r="D2" s="301"/>
-      <c r="E2" s="301"/>
-      <c r="F2" s="301"/>
-      <c r="G2" s="301"/>
-      <c r="H2" s="301"/>
+      <c r="B2" s="290"/>
+      <c r="C2" s="290"/>
+      <c r="D2" s="290"/>
+      <c r="E2" s="290"/>
+      <c r="F2" s="290"/>
+      <c r="G2" s="290"/>
+      <c r="H2" s="290"/>
     </row>
     <row r="3" spans="1:11" s="85" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="84"/>
@@ -10137,12 +9959,12 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C4" s="83"/>
-      <c r="D4" s="286" t="s">
+      <c r="D4" s="273" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="287"/>
+      <c r="E4" s="274"/>
       <c r="F4" s="192"/>
-      <c r="G4" s="284">
+      <c r="G4" s="271">
         <f>Parámetros!E13</f>
         <v>2662</v>
       </c>
@@ -10153,10 +9975,10 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C5" s="83"/>
-      <c r="D5" s="288"/>
-      <c r="E5" s="289"/>
+      <c r="D5" s="275"/>
+      <c r="E5" s="276"/>
       <c r="F5" s="193"/>
-      <c r="G5" s="285"/>
+      <c r="G5" s="272"/>
       <c r="H5" s="28"/>
       <c r="I5" s="28"/>
       <c r="J5" s="28"/>
@@ -10164,12 +9986,12 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C6" s="83"/>
-      <c r="D6" s="286" t="s">
+      <c r="D6" s="273" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="287"/>
+      <c r="E6" s="274"/>
       <c r="F6" s="192"/>
-      <c r="G6" s="284">
+      <c r="G6" s="271">
         <f>Parámetros!E12</f>
         <v>15</v>
       </c>
@@ -10180,10 +10002,10 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C7" s="83"/>
-      <c r="D7" s="288"/>
-      <c r="E7" s="289"/>
+      <c r="D7" s="275"/>
+      <c r="E7" s="276"/>
       <c r="F7" s="193"/>
-      <c r="G7" s="285"/>
+      <c r="G7" s="272"/>
       <c r="H7" s="28"/>
       <c r="I7" s="28"/>
       <c r="J7" s="28"/>
@@ -10191,24 +10013,24 @@
     </row>
     <row r="8" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:11" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="279" t="s">
+      <c r="A9" s="266" t="s">
         <v>63</v>
       </c>
-      <c r="B9" s="279"/>
-      <c r="C9" s="279"/>
-      <c r="D9" s="279"/>
-      <c r="E9" s="279"/>
-      <c r="F9" s="279"/>
-      <c r="G9" s="279"/>
-      <c r="H9" s="279"/>
+      <c r="B9" s="266"/>
+      <c r="C9" s="266"/>
+      <c r="D9" s="266"/>
+      <c r="E9" s="266"/>
+      <c r="F9" s="266"/>
+      <c r="G9" s="266"/>
+      <c r="H9" s="266"/>
     </row>
     <row r="11" spans="1:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="299" t="s">
+      <c r="A12" s="286" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="300"/>
-      <c r="C12" s="300"/>
+      <c r="B12" s="287"/>
+      <c r="C12" s="287"/>
       <c r="D12" s="27" t="s">
         <v>48</v>
       </c>
@@ -10226,11 +10048,11 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="296" t="s">
+      <c r="A13" s="283" t="s">
         <v>55</v>
       </c>
-      <c r="B13" s="297"/>
-      <c r="C13" s="298"/>
+      <c r="B13" s="284"/>
+      <c r="C13" s="285"/>
       <c r="D13" s="61">
         <v>3</v>
       </c>
@@ -10248,11 +10070,11 @@
       <c r="H13" s="96"/>
     </row>
     <row r="14" spans="1:11" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="296" t="s">
+      <c r="A14" s="283" t="s">
         <v>162</v>
       </c>
-      <c r="B14" s="297"/>
-      <c r="C14" s="298"/>
+      <c r="B14" s="284"/>
+      <c r="C14" s="285"/>
       <c r="D14" s="62">
         <v>2</v>
       </c>
@@ -10270,11 +10092,11 @@
       <c r="H14" s="97"/>
     </row>
     <row r="15" spans="1:11" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="296" t="s">
+      <c r="A15" s="283" t="s">
         <v>56</v>
       </c>
-      <c r="B15" s="297"/>
-      <c r="C15" s="298"/>
+      <c r="B15" s="284"/>
+      <c r="C15" s="285"/>
       <c r="D15" s="62">
         <v>3</v>
       </c>
@@ -10292,11 +10114,11 @@
       <c r="H15" s="97"/>
     </row>
     <row r="16" spans="1:11" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="296" t="s">
+      <c r="A16" s="283" t="s">
         <v>57</v>
       </c>
-      <c r="B16" s="297"/>
-      <c r="C16" s="298"/>
+      <c r="B16" s="284"/>
+      <c r="C16" s="285"/>
       <c r="D16" s="62">
         <v>3</v>
       </c>
@@ -10314,11 +10136,11 @@
       <c r="H16" s="97"/>
     </row>
     <row r="17" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="296" t="s">
+      <c r="A17" s="283" t="s">
         <v>58</v>
       </c>
-      <c r="B17" s="297"/>
-      <c r="C17" s="298"/>
+      <c r="B17" s="284"/>
+      <c r="C17" s="285"/>
       <c r="D17" s="62">
         <v>5</v>
       </c>
@@ -10336,11 +10158,11 @@
       <c r="H17" s="97"/>
     </row>
     <row r="18" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="303" t="s">
+      <c r="A18" s="288" t="s">
         <v>163</v>
       </c>
-      <c r="B18" s="303"/>
-      <c r="C18" s="304"/>
+      <c r="B18" s="288"/>
+      <c r="C18" s="289"/>
       <c r="D18" s="62">
         <v>4</v>
       </c>
@@ -10358,11 +10180,11 @@
       <c r="H18" s="97"/>
     </row>
     <row r="19" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="296" t="s">
+      <c r="A19" s="283" t="s">
         <v>164</v>
       </c>
-      <c r="B19" s="297"/>
-      <c r="C19" s="298"/>
+      <c r="B19" s="284"/>
+      <c r="C19" s="285"/>
       <c r="D19" s="65">
         <v>4</v>
       </c>
@@ -10380,11 +10202,11 @@
       <c r="H19" s="98"/>
     </row>
     <row r="20" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="296" t="s">
+      <c r="A20" s="283" t="s">
         <v>59</v>
       </c>
-      <c r="B20" s="297"/>
-      <c r="C20" s="298"/>
+      <c r="B20" s="284"/>
+      <c r="C20" s="285"/>
       <c r="D20" s="65">
         <v>2</v>
       </c>
@@ -10409,6 +10231,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="D4:E5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="D6:E7"/>
+    <mergeCell ref="G6:G7"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="A18:C18"/>
     <mergeCell ref="A20:C20"/>
@@ -10417,14 +10247,6 @@
     <mergeCell ref="A16:C16"/>
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="D4:E5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="D6:E7"/>
-    <mergeCell ref="G6:G7"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.2" right="0.2" top="0.43" bottom="0.4" header="0.17" footer="0.21"/>
@@ -10499,7 +10321,7 @@
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="90" zoomScaleNormal="75" zoomScaleSheetLayoutView="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H15" sqref="H15"/>
+      <selection pane="bottomLeft" sqref="A1:N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -10519,49 +10341,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="257" t="s">
+      <c r="A1" s="250" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="257"/>
-      <c r="C1" s="257"/>
-      <c r="D1" s="257"/>
-      <c r="E1" s="257"/>
-      <c r="F1" s="257"/>
-      <c r="G1" s="257"/>
-      <c r="H1" s="257"/>
-      <c r="I1" s="257"/>
-      <c r="J1" s="257"/>
-      <c r="K1" s="257"/>
-      <c r="L1" s="257"/>
-      <c r="M1" s="257"/>
-      <c r="N1" s="257"/>
+      <c r="B1" s="250"/>
+      <c r="C1" s="250"/>
+      <c r="D1" s="250"/>
+      <c r="E1" s="250"/>
+      <c r="F1" s="250"/>
+      <c r="G1" s="250"/>
+      <c r="H1" s="250"/>
+      <c r="I1" s="250"/>
+      <c r="J1" s="250"/>
+      <c r="K1" s="250"/>
+      <c r="L1" s="250"/>
+      <c r="M1" s="250"/>
+      <c r="N1" s="250"/>
     </row>
     <row r="2" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="257" t="s">
+      <c r="A2" s="250" t="s">
         <v>90</v>
       </c>
-      <c r="B2" s="257"/>
-      <c r="C2" s="257"/>
-      <c r="D2" s="257"/>
-      <c r="E2" s="257"/>
-      <c r="F2" s="257"/>
-      <c r="G2" s="257"/>
-      <c r="H2" s="257"/>
-      <c r="I2" s="257"/>
-      <c r="J2" s="257"/>
-      <c r="K2" s="257"/>
-      <c r="L2" s="257"/>
-      <c r="M2" s="257"/>
-      <c r="N2" s="257"/>
+      <c r="B2" s="250"/>
+      <c r="C2" s="250"/>
+      <c r="D2" s="250"/>
+      <c r="E2" s="250"/>
+      <c r="F2" s="250"/>
+      <c r="G2" s="250"/>
+      <c r="H2" s="250"/>
+      <c r="I2" s="250"/>
+      <c r="J2" s="250"/>
+      <c r="K2" s="250"/>
+      <c r="L2" s="250"/>
+      <c r="M2" s="250"/>
+      <c r="N2" s="250"/>
     </row>
     <row r="3" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:14" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C4" s="83"/>
-      <c r="D4" s="286" t="s">
+      <c r="D4" s="273" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="287"/>
-      <c r="F4" s="284">
+      <c r="E4" s="274"/>
+      <c r="F4" s="271">
         <f>Parámetros!E13</f>
         <v>2662</v>
       </c>
@@ -10572,9 +10394,9 @@
     </row>
     <row r="5" spans="1:14" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C5" s="83"/>
-      <c r="D5" s="288"/>
-      <c r="E5" s="289"/>
-      <c r="F5" s="285"/>
+      <c r="D5" s="275"/>
+      <c r="E5" s="276"/>
+      <c r="F5" s="272"/>
       <c r="G5" s="28"/>
       <c r="H5" s="28"/>
       <c r="I5" s="28"/>
@@ -10582,11 +10404,11 @@
     </row>
     <row r="6" spans="1:14" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C6" s="83"/>
-      <c r="D6" s="286" t="s">
+      <c r="D6" s="273" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="287"/>
-      <c r="F6" s="284">
+      <c r="E6" s="274"/>
+      <c r="F6" s="271">
         <f>Parámetros!E12</f>
         <v>15</v>
       </c>
@@ -10597,9 +10419,9 @@
     </row>
     <row r="7" spans="1:14" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C7" s="83"/>
-      <c r="D7" s="288"/>
-      <c r="E7" s="289"/>
-      <c r="F7" s="285"/>
+      <c r="D7" s="275"/>
+      <c r="E7" s="276"/>
+      <c r="F7" s="272"/>
       <c r="G7" s="28"/>
       <c r="H7" s="28"/>
       <c r="I7" s="28"/>
@@ -10618,24 +10440,24 @@
       <c r="J10" s="9"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B11" s="305" t="s">
+      <c r="B11" s="292" t="s">
         <v>92</v>
       </c>
-      <c r="C11" s="311"/>
-      <c r="D11" s="312"/>
-      <c r="H11" s="305" t="s">
+      <c r="C11" s="298"/>
+      <c r="D11" s="299"/>
+      <c r="H11" s="292" t="s">
         <v>93</v>
       </c>
-      <c r="I11" s="306"/>
-      <c r="J11" s="307"/>
+      <c r="I11" s="293"/>
+      <c r="J11" s="294"/>
     </row>
     <row r="12" spans="1:14" ht="13.2" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="313"/>
-      <c r="C12" s="314"/>
-      <c r="D12" s="315"/>
-      <c r="H12" s="308"/>
-      <c r="I12" s="309"/>
-      <c r="J12" s="310"/>
+      <c r="B12" s="300"/>
+      <c r="C12" s="301"/>
+      <c r="D12" s="302"/>
+      <c r="H12" s="295"/>
+      <c r="I12" s="296"/>
+      <c r="J12" s="297"/>
     </row>
     <row r="13" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="91" t="s">
@@ -10884,7 +10706,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -10895,28 +10717,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="257" t="s">
+      <c r="A1" s="250" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="257"/>
-      <c r="C1" s="257"/>
-      <c r="D1" s="257"/>
-      <c r="E1" s="257"/>
-      <c r="F1" s="257"/>
-      <c r="G1" s="257"/>
-      <c r="H1" s="257"/>
+      <c r="B1" s="250"/>
+      <c r="C1" s="250"/>
+      <c r="D1" s="250"/>
+      <c r="E1" s="250"/>
+      <c r="F1" s="250"/>
+      <c r="G1" s="250"/>
+      <c r="H1" s="250"/>
     </row>
     <row r="2" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A2" s="257" t="s">
+      <c r="A2" s="250" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="257"/>
-      <c r="C2" s="257"/>
-      <c r="D2" s="257"/>
-      <c r="E2" s="257"/>
-      <c r="F2" s="257"/>
-      <c r="G2" s="257"/>
-      <c r="H2" s="257"/>
+      <c r="B2" s="250"/>
+      <c r="C2" s="250"/>
+      <c r="D2" s="250"/>
+      <c r="E2" s="250"/>
+      <c r="F2" s="250"/>
+      <c r="G2" s="250"/>
+      <c r="H2" s="250"/>
     </row>
     <row r="5" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="103" t="s">
@@ -10943,15 +10765,15 @@
         <v>32</v>
       </c>
       <c r="B6" s="25">
-        <f>Actores!C36</f>
+        <f>Actores!C19</f>
         <v>0</v>
       </c>
       <c r="C6" s="25">
-        <f>Actores!D36</f>
+        <f>Actores!D19</f>
         <v>0</v>
       </c>
       <c r="D6" s="25">
-        <f>Actores!E36</f>
+        <f>Actores!E19</f>
         <v>3</v>
       </c>
       <c r="E6" s="25">
@@ -10984,25 +10806,25 @@
       <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="316">
+      <c r="B8" s="303">
         <f>(0.65+(0.01*'Ajustes Técnicos'!E26))</f>
         <v>1.07</v>
       </c>
-      <c r="C8" s="317"/>
-      <c r="D8" s="317"/>
-      <c r="E8" s="318"/>
+      <c r="C8" s="304"/>
+      <c r="D8" s="304"/>
+      <c r="E8" s="305"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="316">
+      <c r="B9" s="303">
         <f>(1.3375+ (-0.03 *'Ajustes Ambientales'!G21))</f>
         <v>1.3374999999999999</v>
       </c>
-      <c r="C9" s="317"/>
-      <c r="D9" s="317"/>
-      <c r="E9" s="318"/>
+      <c r="C9" s="304"/>
+      <c r="D9" s="304"/>
+      <c r="E9" s="305"/>
     </row>
     <row r="10" spans="1:8" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -11018,7 +10840,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="324" t="s">
+      <c r="A12" s="210" t="s">
         <v>33</v>
       </c>
       <c r="B12" s="68"/>
@@ -11159,29 +10981,29 @@
       <c r="AF2" s="182"/>
       <c r="AG2" s="182"/>
       <c r="AH2" s="182"/>
-      <c r="AI2" s="223" t="s">
+      <c r="AI2" s="322" t="s">
         <v>27</v>
       </c>
-      <c r="AJ2" s="223"/>
-      <c r="AK2" s="224" t="s">
+      <c r="AJ2" s="322"/>
+      <c r="AK2" s="323" t="s">
         <v>106</v>
       </c>
-      <c r="AL2" s="224"/>
-      <c r="AM2" s="224"/>
-      <c r="AN2" s="222"/>
-      <c r="AO2" s="222"/>
-      <c r="AP2" s="222"/>
-      <c r="AQ2" s="222"/>
-      <c r="AR2" s="222"/>
-      <c r="AS2" s="222"/>
-      <c r="AT2" s="221"/>
-      <c r="AU2" s="221"/>
-      <c r="AV2" s="221"/>
-      <c r="AW2" s="221"/>
-      <c r="AX2" s="221"/>
-      <c r="AY2" s="221"/>
-      <c r="AZ2" s="221"/>
-      <c r="BA2" s="221"/>
+      <c r="AL2" s="323"/>
+      <c r="AM2" s="323"/>
+      <c r="AN2" s="321"/>
+      <c r="AO2" s="321"/>
+      <c r="AP2" s="321"/>
+      <c r="AQ2" s="321"/>
+      <c r="AR2" s="321"/>
+      <c r="AS2" s="321"/>
+      <c r="AT2" s="320"/>
+      <c r="AU2" s="320"/>
+      <c r="AV2" s="320"/>
+      <c r="AW2" s="320"/>
+      <c r="AX2" s="320"/>
+      <c r="AY2" s="320"/>
+      <c r="AZ2" s="320"/>
+      <c r="BA2" s="320"/>
       <c r="BB2" s="124"/>
       <c r="BC2" s="124"/>
     </row>
@@ -13669,19 +13491,19 @@
     </row>
     <row r="26" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A26" s="133"/>
-      <c r="B26" s="207" t="s">
+      <c r="B26" s="306" t="s">
         <v>92</v>
       </c>
-      <c r="C26" s="216"/>
-      <c r="D26" s="217"/>
+      <c r="C26" s="315"/>
+      <c r="D26" s="316"/>
       <c r="AL26" s="125"/>
       <c r="BA26" s="132"/>
     </row>
     <row r="27" spans="1:67" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="133"/>
-      <c r="B27" s="218"/>
-      <c r="C27" s="219"/>
-      <c r="D27" s="220"/>
+      <c r="B27" s="317"/>
+      <c r="C27" s="318"/>
+      <c r="D27" s="319"/>
       <c r="E27" s="122" t="s">
         <v>121</v>
       </c>
@@ -14115,11 +13937,11 @@
       <c r="K43" s="149"/>
     </row>
     <row r="44" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B44" s="207" t="s">
+      <c r="B44" s="306" t="s">
         <v>125</v>
       </c>
-      <c r="C44" s="216"/>
-      <c r="D44" s="217"/>
+      <c r="C44" s="315"/>
+      <c r="D44" s="316"/>
       <c r="E44" s="150" t="s">
         <v>126</v>
       </c>
@@ -14135,14 +13957,14 @@
       <c r="K44" s="149"/>
     </row>
     <row r="45" spans="2:18" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="218" t="s">
+      <c r="B45" s="317" t="s">
         <v>129</v>
       </c>
-      <c r="C45" s="219">
+      <c r="C45" s="318">
         <f>D33</f>
         <v>547.83960000000013</v>
       </c>
-      <c r="D45" s="220"/>
+      <c r="D45" s="319"/>
       <c r="E45" s="151" t="s">
         <v>105</v>
       </c>
@@ -14327,23 +14149,23 @@
       <c r="K54" s="149"/>
     </row>
     <row r="55" spans="2:11" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="207" t="s">
+      <c r="B55" s="306" t="s">
         <v>93</v>
       </c>
-      <c r="C55" s="208"/>
-      <c r="D55" s="209"/>
+      <c r="C55" s="307"/>
+      <c r="D55" s="308"/>
     </row>
     <row r="56" spans="2:11" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="210">
-        <v>0</v>
-      </c>
-      <c r="C56" s="211"/>
-      <c r="D56" s="212"/>
-      <c r="E56" s="213" t="s">
+      <c r="B56" s="309">
+        <v>0</v>
+      </c>
+      <c r="C56" s="310"/>
+      <c r="D56" s="311"/>
+      <c r="E56" s="312" t="s">
         <v>126</v>
       </c>
-      <c r="F56" s="214"/>
-      <c r="G56" s="215"/>
+      <c r="F56" s="313"/>
+      <c r="G56" s="314"/>
     </row>
     <row r="57" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B57" s="154" t="s">
@@ -14355,11 +14177,11 @@
       <c r="D57" s="156" t="s">
         <v>11</v>
       </c>
-      <c r="E57" s="213" t="s">
+      <c r="E57" s="312" t="s">
         <v>3</v>
       </c>
-      <c r="F57" s="214"/>
-      <c r="G57" s="215"/>
+      <c r="F57" s="313"/>
+      <c r="G57" s="314"/>
     </row>
     <row r="58" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B58" s="134" t="str">

</xml_diff>